<commit_message>
Update for survey_round 44 UK data
</commit_message>
<xml_diff>
--- a/data/spss_uk.xlsx
+++ b/data/spss_uk.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34BA811-C0DE-4CE8-95EE-D71B5362FB59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3531EAAF-1F27-49E5-8EA9-52D2FC27C2B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{B6B7C775-E4A7-4345-8BD6-E691E151534C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6B7C775-E4A7-4345-8BD6-E691E151534C}"/>
   </bookViews>
   <sheets>
     <sheet name="UK" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="81">
   <si>
     <t>survey_version</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t>20-100562_PEW13_Final</t>
+  </si>
+  <si>
+    <t>20-100590_PFW13_Final_ICUO</t>
   </si>
 </sst>
 </file>
@@ -626,22 +629,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E8812C-49CD-4565-ACAD-8E318F9F9624}">
-  <dimension ref="A1:O56"/>
+  <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48:K57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.3828125" customWidth="1"/>
-    <col min="7" max="7" width="10.69140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="58.3046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.3046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="58.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -688,7 +691,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -714,7 +717,7 @@
         <v>17</v>
       </c>
       <c r="I2" t="str">
-        <f t="shared" ref="I2:I56" si="0">C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
+        <f t="shared" ref="I2:I57" si="0">C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
         <v>uk_wk01_20200402_pA_wv01</v>
       </c>
       <c r="J2">
@@ -724,7 +727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -760,7 +763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -796,7 +799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -832,7 +835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -868,7 +871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -904,7 +907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -943,7 +946,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -979,7 +982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1016,7 +1019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1053,7 +1056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1090,7 +1093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1128,7 +1131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1165,7 +1168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1202,7 +1205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1239,7 +1242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1276,7 +1279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1313,7 +1316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1350,7 +1353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1387,7 +1390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1424,7 +1427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1461,7 +1464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1498,7 +1501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1535,7 +1538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1572,7 +1575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1609,7 +1612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1646,7 +1649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1686,7 +1689,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1726,7 +1729,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1763,7 +1766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1799,7 +1802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1838,7 +1841,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1874,7 +1877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3</v>
       </c>
@@ -1891,7 +1894,7 @@
         <v>52</v>
       </c>
       <c r="F34">
-        <f t="shared" ref="F34:F56" si="4">F32+1</f>
+        <f t="shared" ref="F34:F57" si="4">F32+1</f>
         <v>2</v>
       </c>
       <c r="G34" s="1">
@@ -1911,7 +1914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3</v>
       </c>
@@ -1948,7 +1951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>3</v>
       </c>
@@ -1985,7 +1988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>3</v>
       </c>
@@ -2022,7 +2025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3</v>
       </c>
@@ -2059,7 +2062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3</v>
       </c>
@@ -2096,7 +2099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2133,7 +2136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>3</v>
       </c>
@@ -2170,7 +2173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2207,7 +2210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2244,7 +2247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>3</v>
       </c>
@@ -2277,8 +2280,11 @@
       <c r="J44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>3</v>
       </c>
@@ -2315,7 +2321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>3</v>
       </c>
@@ -2352,7 +2358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>3</v>
       </c>
@@ -2389,7 +2395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>3</v>
       </c>
@@ -2422,8 +2428,11 @@
       <c r="J48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>3</v>
       </c>
@@ -2456,8 +2465,11 @@
       <c r="J49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>3</v>
       </c>
@@ -2490,8 +2502,11 @@
       <c r="J50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>3</v>
       </c>
@@ -2524,8 +2539,11 @@
       <c r="J51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>3</v>
       </c>
@@ -2558,8 +2576,11 @@
       <c r="J52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>3</v>
       </c>
@@ -2592,8 +2613,11 @@
       <c r="J53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>3</v>
       </c>
@@ -2626,8 +2650,11 @@
       <c r="J54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>3</v>
       </c>
@@ -2660,8 +2687,11 @@
       <c r="J55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>3</v>
       </c>
@@ -2692,6 +2722,46 @@
         <v>uk_wk44_20210128_pE_wv13</v>
       </c>
       <c r="J56">
+        <v>1</v>
+      </c>
+      <c r="K56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>3</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57">
+        <v>45</v>
+      </c>
+      <c r="E57" t="s">
+        <v>55</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="G57" s="1">
+        <v>44232</v>
+      </c>
+      <c r="H57" t="s">
+        <v>80</v>
+      </c>
+      <c r="I57" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_wk45_20210205_pF_wv13</v>
+      </c>
+      <c r="J57">
+        <v>1</v>
+      </c>
+      <c r="K57">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update with UK name in a seperate shee
</commit_message>
<xml_diff>
--- a/data/spss_uk.xlsx
+++ b/data/spss_uk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1313C0D4-6FBC-4789-9F92-574E67925D9D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4CB95A-9734-4CBB-A292-CD4A24297392}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6B7C775-E4A7-4345-8BD6-E691E151534C}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{B6B7C775-E4A7-4345-8BD6-E691E151534C}"/>
   </bookViews>
   <sheets>
     <sheet name="UK" sheetId="1" r:id="rId1"/>
@@ -632,19 +632,19 @@
   <dimension ref="A1:O57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="K48" sqref="K48:K57"/>
+      <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="58.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3828125" customWidth="1"/>
+    <col min="7" max="7" width="10.69140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="58.3046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -691,7 +691,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -727,7 +727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -763,7 +763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1</v>
       </c>
@@ -799,7 +799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1</v>
       </c>
@@ -835,7 +835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>1</v>
       </c>
@@ -871,7 +871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>1</v>
       </c>
@@ -907,7 +907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>1</v>
       </c>
@@ -946,7 +946,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>2</v>
       </c>
@@ -982,7 +982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1093,7 +1093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1877,7 +1877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>3</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>3</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>3</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>3</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>3</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A39">
         <v>3</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>3</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2247,7 +2247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A44">
         <v>3</v>
       </c>
@@ -2284,7 +2284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A45">
         <v>3</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A46">
         <v>3</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A47">
         <v>3</v>
       </c>
@@ -2395,7 +2395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A48">
         <v>3</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A49">
         <v>3</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>3</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A51">
         <v>3</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A52">
         <v>3</v>
       </c>
@@ -2580,7 +2580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A53">
         <v>3</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A54">
         <v>3</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A55">
         <v>3</v>
       </c>
@@ -2691,7 +2691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A56">
         <v>3</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A57">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Updated for latest UK data
</commit_message>
<xml_diff>
--- a/data/spss_uk.xlsx
+++ b/data/spss_uk.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4CB95A-9734-4CBB-A292-CD4A24297392}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC0B245C-0EB1-411A-99CC-05755FCE1782}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{B6B7C775-E4A7-4345-8BD6-E691E151534C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="83">
   <si>
     <t>survey_version</t>
   </si>
@@ -276,7 +276,13 @@
     <t>20-100562_PEW13_Final</t>
   </si>
   <si>
-    <t>20-100590_PFW13_Final_ICUO</t>
+    <t>20-100562_PEW14_Final_ICUO_V2</t>
+  </si>
+  <si>
+    <t>20-100590_PFW13_Final_IntUseV2</t>
+  </si>
+  <si>
+    <t>Update as people were not asked vaccine questions</t>
   </si>
 </sst>
 </file>
@@ -629,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E8812C-49CD-4565-ACAD-8E318F9F9624}">
-  <dimension ref="A1:O57"/>
+  <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="I57" sqref="I57"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1894,7 +1900,7 @@
         <v>52</v>
       </c>
       <c r="F34">
-        <f t="shared" ref="F34:F57" si="4">F32+1</f>
+        <f t="shared" ref="F34:F59" si="4">F32+1</f>
         <v>2</v>
       </c>
       <c r="G34" s="1">
@@ -2432,7 +2438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A49">
         <v>3</v>
       </c>
@@ -2469,7 +2475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>3</v>
       </c>
@@ -2506,7 +2512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A51">
         <v>3</v>
       </c>
@@ -2543,7 +2549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A52">
         <v>3</v>
       </c>
@@ -2580,7 +2586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A53">
         <v>3</v>
       </c>
@@ -2617,7 +2623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A54">
         <v>3</v>
       </c>
@@ -2654,7 +2660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A55">
         <v>3</v>
       </c>
@@ -2691,7 +2697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A56">
         <v>3</v>
       </c>
@@ -2728,7 +2734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A57">
         <v>3</v>
       </c>
@@ -2752,16 +2758,56 @@
         <v>44232</v>
       </c>
       <c r="H57" t="s">
+        <v>81</v>
+      </c>
+      <c r="I57" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_wk45_20210205_pF_wv13</v>
+      </c>
+      <c r="J57">
+        <v>1</v>
+      </c>
+      <c r="K57">
+        <v>1</v>
+      </c>
+      <c r="O57" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A58">
+        <v>3</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58">
+        <v>46</v>
+      </c>
+      <c r="E58" t="s">
+        <v>52</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="G58" s="1">
+        <v>44246</v>
+      </c>
+      <c r="H58" t="s">
         <v>80</v>
       </c>
-      <c r="I57" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk45_20210205_pF_wv13</v>
-      </c>
-      <c r="J57">
-        <v>1</v>
-      </c>
-      <c r="K57">
+      <c r="I58" t="str">
+        <f t="shared" ref="I58" si="5">C58&amp;"_"&amp;"wk"&amp;TEXT(D58,"00")&amp;"_"&amp;YEAR(G58)&amp;TEXT(G58,"MM")&amp;TEXT(G58,"DD")&amp;"_p"&amp;E58&amp;"_wv"&amp;TEXT(F58,"00")&amp;""</f>
+        <v>uk_wk46_20210219_pE_wv14</v>
+      </c>
+      <c r="J58">
+        <v>1</v>
+      </c>
+      <c r="K58">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update for latest panel
</commit_message>
<xml_diff>
--- a/data/spss_uk.xlsx
+++ b/data/spss_uk.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265AE563-B300-4B39-881D-365E044EB8D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1308EC-BB8C-493C-9973-DADF8962302D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{B6B7C775-E4A7-4345-8BD6-E691E151534C}"/>
   </bookViews>
@@ -288,7 +288,7 @@
     <t>20-100562_PEW15_Final_ICUO</t>
   </si>
   <si>
-    <t>20-100590-PFW13_final_combined.sav</t>
+    <t>20-100590-PFW13_final_combined</t>
   </si>
 </sst>
 </file>
@@ -644,7 +644,7 @@
   <dimension ref="A1:O60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H57" sqref="H57"/>
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Update UK data for Panel F15 sr 49
</commit_message>
<xml_diff>
--- a/data/spss_uk.xlsx
+++ b/data/spss_uk.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4553E03C-EF2D-4CCA-8ED9-3E05640E7D27}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B440B9B-0142-4560-ABB9-9F84345F4060}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{B6B7C775-E4A7-4345-8BD6-E691E151534C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="86">
   <si>
     <t>survey_version</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>survey_round</t>
+  </si>
+  <si>
+    <t>20-100590_PFW15_Final_IntUse_nodups</t>
   </si>
 </sst>
 </file>
@@ -641,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E8812C-49CD-4565-ACAD-8E318F9F9624}">
-  <dimension ref="A1:O60"/>
+  <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:I60"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -765,7 +768,7 @@
         <v>18</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I60" si="0">C3&amp;"_"&amp;"sr"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
+        <f t="shared" ref="I3:I61" si="0">C3&amp;"_"&amp;"sr"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
         <v>uk_sr02_20200214_pB_wv01</v>
       </c>
       <c r="J3">
@@ -1906,7 +1909,7 @@
         <v>51</v>
       </c>
       <c r="F34">
-        <f t="shared" ref="F34:F58" si="4">F32+1</f>
+        <f t="shared" ref="F34:F60" si="4">F32+1</f>
         <v>2</v>
       </c>
       <c r="G34" s="1">
@@ -2870,6 +2873,7 @@
         <v>51</v>
       </c>
       <c r="F60">
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="G60" s="1">
@@ -2883,6 +2887,39 @@
         <v>uk_sr48_20210225_pE_wv15</v>
       </c>
       <c r="J60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A61">
+        <v>3</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61">
+        <v>49</v>
+      </c>
+      <c r="E61" t="s">
+        <v>54</v>
+      </c>
+      <c r="F61">
+        <v>15</v>
+      </c>
+      <c r="G61" s="1">
+        <v>44259</v>
+      </c>
+      <c r="H61" t="s">
+        <v>85</v>
+      </c>
+      <c r="I61" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr49_20210304_pF_wv15</v>
+      </c>
+      <c r="J61">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update for round 52 of UK data
</commit_message>
<xml_diff>
--- a/data/spss_uk.xlsx
+++ b/data/spss_uk.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amygimma/lshtm/comix_data_clean/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E568B1-0F84-AB47-B818-9F27DFA9B0A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C362BF-5EE4-4374-8E7A-16F6041605B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{B6B7C775-E4A7-4345-8BD6-E691E151534C}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{B6B7C775-E4A7-4345-8BD6-E691E151534C}"/>
   </bookViews>
   <sheets>
     <sheet name="UK" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="89">
   <si>
     <t>survey_version</t>
   </si>
@@ -298,6 +298,9 @@
   </si>
   <si>
     <t>20-100562_PEW16_Final_ICUO</t>
+  </si>
+  <si>
+    <t>20-100562_PEW17_Final_ICUO</t>
   </si>
 </sst>
 </file>
@@ -650,22 +653,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E8812C-49CD-4565-ACAD-8E318F9F9624}">
-  <dimension ref="A1:O63"/>
+  <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J64" sqref="J64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="58.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3046875" customWidth="1"/>
+    <col min="7" max="7" width="10.69140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="58.3046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -712,7 +715,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -748,7 +751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -774,7 +777,7 @@
         <v>18</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I63" si="0">C3&amp;"_"&amp;"sr"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
+        <f t="shared" ref="I3:I64" si="0">C3&amp;"_"&amp;"sr"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
         <v>uk_sr02_20200214_pB_wv01</v>
       </c>
       <c r="J3">
@@ -784,7 +787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1</v>
       </c>
@@ -820,7 +823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1</v>
       </c>
@@ -856,7 +859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>1</v>
       </c>
@@ -892,7 +895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>1</v>
       </c>
@@ -928,7 +931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>1</v>
       </c>
@@ -967,7 +970,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1003,7 +1006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1040,7 +1043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1077,7 +1080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1114,7 +1117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1152,7 +1155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1189,7 +1192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1226,7 +1229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1263,7 +1266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1300,7 +1303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1337,7 +1340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1374,7 +1377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1411,7 +1414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1448,7 +1451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1485,7 +1488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1522,7 +1525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1559,7 +1562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1596,7 +1599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1633,7 +1636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1670,7 +1673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1710,7 +1713,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1750,7 +1753,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1787,7 +1790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1823,7 +1826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1862,7 +1865,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1898,7 +1901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>3</v>
       </c>
@@ -1935,7 +1938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>3</v>
       </c>
@@ -1972,7 +1975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>3</v>
       </c>
@@ -2009,7 +2012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>3</v>
       </c>
@@ -2046,7 +2049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>3</v>
       </c>
@@ -2083,7 +2086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A39">
         <v>3</v>
       </c>
@@ -2120,7 +2123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2157,7 +2160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>3</v>
       </c>
@@ -2194,7 +2197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2231,7 +2234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2268,7 +2271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A44">
         <v>3</v>
       </c>
@@ -2305,7 +2308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A45">
         <v>3</v>
       </c>
@@ -2342,7 +2345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A46">
         <v>3</v>
       </c>
@@ -2379,7 +2382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A47">
         <v>3</v>
       </c>
@@ -2416,7 +2419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A48">
         <v>3</v>
       </c>
@@ -2453,7 +2456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A49">
         <v>3</v>
       </c>
@@ -2490,7 +2493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>3</v>
       </c>
@@ -2527,7 +2530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A51">
         <v>3</v>
       </c>
@@ -2564,7 +2567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A52">
         <v>3</v>
       </c>
@@ -2601,7 +2604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A53">
         <v>3</v>
       </c>
@@ -2638,7 +2641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A54">
         <v>3</v>
       </c>
@@ -2675,7 +2678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A55">
         <v>3</v>
       </c>
@@ -2712,7 +2715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A56">
         <v>3</v>
       </c>
@@ -2749,7 +2752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A57">
         <v>3</v>
       </c>
@@ -2789,7 +2792,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A58">
         <v>3</v>
       </c>
@@ -2826,7 +2829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A59">
         <v>3</v>
       </c>
@@ -2862,7 +2865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A60">
         <v>3</v>
       </c>
@@ -2895,9 +2898,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A61">
         <v>3</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
       </c>
       <c r="C61" t="s">
         <v>14</v>
@@ -2921,10 +2927,16 @@
         <f t="shared" si="0"/>
         <v>uk_sr49_20210305_pF_wv15</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A62">
         <v>3</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
       </c>
       <c r="C62" t="s">
         <v>14</v>
@@ -2948,10 +2960,16 @@
         <f t="shared" si="0"/>
         <v>uk_sr50_20210312_pE_wv16</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A63">
         <v>3</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
       </c>
       <c r="C63" t="s">
         <v>14</v>
@@ -2974,6 +2992,42 @@
       <c r="I63" t="str">
         <f t="shared" si="0"/>
         <v>uk_sr51_20210319_pF_wv16</v>
+      </c>
+      <c r="J63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A64">
+        <v>3</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64" t="s">
+        <v>14</v>
+      </c>
+      <c r="D64">
+        <v>52</v>
+      </c>
+      <c r="E64" t="s">
+        <v>51</v>
+      </c>
+      <c r="F64">
+        <v>17</v>
+      </c>
+      <c r="G64" s="1">
+        <v>44284</v>
+      </c>
+      <c r="H64" t="s">
+        <v>88</v>
+      </c>
+      <c r="I64" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr52_20210329_pE_wv17</v>
+      </c>
+      <c r="J64">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for latest UK data survey round 56
</commit_message>
<xml_diff>
--- a/data/spss_uk.xlsx
+++ b/data/spss_uk.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C362BF-5EE4-4374-8E7A-16F6041605B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B4B9A7F-5AC1-4AC5-8F38-E5F5909E982D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{B6B7C775-E4A7-4345-8BD6-E691E151534C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6B7C775-E4A7-4345-8BD6-E691E151534C}"/>
   </bookViews>
   <sheets>
     <sheet name="UK" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="93">
   <si>
     <t>survey_version</t>
   </si>
@@ -301,6 +301,18 @@
   </si>
   <si>
     <t>20-100562_PEW17_Final_ICUO</t>
+  </si>
+  <si>
+    <t>20-100590_PFW17_Final_ICUO</t>
+  </si>
+  <si>
+    <t>20-100562_PEW18_Final_ICUO</t>
+  </si>
+  <si>
+    <t>20-100590_PFW18_Final_ICUO</t>
+  </si>
+  <si>
+    <t>20-100562_PEW19_Final_ICUO</t>
   </si>
 </sst>
 </file>
@@ -653,22 +665,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E8812C-49CD-4565-ACAD-8E318F9F9624}">
-  <dimension ref="A1:O64"/>
+  <dimension ref="A1:O68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="J64" sqref="J64"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="J68" sqref="J68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.3046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.3046875" customWidth="1"/>
-    <col min="7" max="7" width="10.69140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="58.3046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.3046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="58.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -715,7 +727,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -751,7 +763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -777,7 +789,7 @@
         <v>18</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I64" si="0">C3&amp;"_"&amp;"sr"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
+        <f t="shared" ref="I3:I68" si="0">C3&amp;"_"&amp;"sr"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
         <v>uk_sr02_20200214_pB_wv01</v>
       </c>
       <c r="J3">
@@ -787,7 +799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -823,7 +835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -859,7 +871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -895,7 +907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -931,7 +943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -970,7 +982,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1006,7 +1018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1043,7 +1055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1080,7 +1092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1117,7 +1129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1155,7 +1167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1192,7 +1204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1229,7 +1241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1266,7 +1278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1303,7 +1315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1340,7 +1352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1377,7 +1389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1414,7 +1426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1451,7 +1463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1488,7 +1500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1525,7 +1537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1562,7 +1574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1599,7 +1611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1636,7 +1648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1673,7 +1685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1713,7 +1725,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1753,7 +1765,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1790,7 +1802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1826,7 +1838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1865,7 +1877,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1901,7 +1913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3</v>
       </c>
@@ -1938,7 +1950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3</v>
       </c>
@@ -1975,7 +1987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>3</v>
       </c>
@@ -2012,7 +2024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>3</v>
       </c>
@@ -2049,7 +2061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3</v>
       </c>
@@ -2086,7 +2098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3</v>
       </c>
@@ -2123,7 +2135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2160,7 +2172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>3</v>
       </c>
@@ -2197,7 +2209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2234,7 +2246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2271,7 +2283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>3</v>
       </c>
@@ -2308,7 +2320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>3</v>
       </c>
@@ -2345,7 +2357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>3</v>
       </c>
@@ -2382,7 +2394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>3</v>
       </c>
@@ -2419,7 +2431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>3</v>
       </c>
@@ -2456,7 +2468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>3</v>
       </c>
@@ -2493,7 +2505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>3</v>
       </c>
@@ -2530,7 +2542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>3</v>
       </c>
@@ -2567,7 +2579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>3</v>
       </c>
@@ -2604,7 +2616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>3</v>
       </c>
@@ -2641,7 +2653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>3</v>
       </c>
@@ -2678,7 +2690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>3</v>
       </c>
@@ -2715,7 +2727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>3</v>
       </c>
@@ -2752,7 +2764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>3</v>
       </c>
@@ -2792,7 +2804,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>3</v>
       </c>
@@ -2829,7 +2841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>3</v>
       </c>
@@ -2865,7 +2877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>3</v>
       </c>
@@ -2898,7 +2910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>3</v>
       </c>
@@ -2931,7 +2943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>3</v>
       </c>
@@ -2964,7 +2976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>3</v>
       </c>
@@ -2997,7 +3009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>3</v>
       </c>
@@ -3027,6 +3039,138 @@
         <v>uk_sr52_20210329_pE_wv17</v>
       </c>
       <c r="J64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>3</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65" t="s">
+        <v>14</v>
+      </c>
+      <c r="D65">
+        <v>53</v>
+      </c>
+      <c r="E65" t="s">
+        <v>54</v>
+      </c>
+      <c r="F65">
+        <v>17</v>
+      </c>
+      <c r="G65" s="1">
+        <v>44292</v>
+      </c>
+      <c r="H65" t="s">
+        <v>89</v>
+      </c>
+      <c r="I65" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr53_20210406_pF_wv17</v>
+      </c>
+      <c r="J65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>3</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66" t="s">
+        <v>14</v>
+      </c>
+      <c r="D66">
+        <v>54</v>
+      </c>
+      <c r="E66" t="s">
+        <v>51</v>
+      </c>
+      <c r="F66">
+        <v>18</v>
+      </c>
+      <c r="G66" s="1">
+        <v>44295</v>
+      </c>
+      <c r="H66" t="s">
+        <v>90</v>
+      </c>
+      <c r="I66" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr54_20210409_pE_wv18</v>
+      </c>
+      <c r="J66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>3</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67" t="s">
+        <v>14</v>
+      </c>
+      <c r="D67">
+        <v>55</v>
+      </c>
+      <c r="E67" t="s">
+        <v>54</v>
+      </c>
+      <c r="F67">
+        <v>18</v>
+      </c>
+      <c r="G67" s="1">
+        <v>44301</v>
+      </c>
+      <c r="H67" t="s">
+        <v>91</v>
+      </c>
+      <c r="I67" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr55_20210415_pF_wv18</v>
+      </c>
+      <c r="J67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>3</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+      <c r="C68" t="s">
+        <v>14</v>
+      </c>
+      <c r="D68">
+        <v>56</v>
+      </c>
+      <c r="E68" t="s">
+        <v>51</v>
+      </c>
+      <c r="F68">
+        <v>19</v>
+      </c>
+      <c r="G68" s="1">
+        <v>44308</v>
+      </c>
+      <c r="H68" t="s">
+        <v>92</v>
+      </c>
+      <c r="I68" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr56_20210422_pE_wv19</v>
+      </c>
+      <c r="J68">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update for latest UK data
</commit_message>
<xml_diff>
--- a/data/spss_uk.xlsx
+++ b/data/spss_uk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B4B9A7F-5AC1-4AC5-8F38-E5F5909E982D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1092E5-51CD-46F9-B25F-3EA6F893BA14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6B7C775-E4A7-4345-8BD6-E691E151534C}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{B6B7C775-E4A7-4345-8BD6-E691E151534C}"/>
   </bookViews>
   <sheets>
     <sheet name="UK" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="94">
   <si>
     <t>survey_version</t>
   </si>
@@ -312,7 +312,10 @@
     <t>20-100590_PFW18_Final_ICUO</t>
   </si>
   <si>
-    <t>20-100562_PEW19_Final_ICUO</t>
+    <t>20-100562_PEW19_Final_ICUO_V2</t>
+  </si>
+  <si>
+    <t>20-100590_PFW19_Final_ICUO</t>
   </si>
 </sst>
 </file>
@@ -665,22 +668,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E8812C-49CD-4565-ACAD-8E318F9F9624}">
-  <dimension ref="A1:O68"/>
+  <dimension ref="A1:O69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="J68" sqref="J68"/>
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="58.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3046875" customWidth="1"/>
+    <col min="7" max="7" width="10.69140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="58.3046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -727,7 +730,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -763,7 +766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -789,7 +792,7 @@
         <v>18</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I68" si="0">C3&amp;"_"&amp;"sr"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
+        <f t="shared" ref="I3:I69" si="0">C3&amp;"_"&amp;"sr"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
         <v>uk_sr02_20200214_pB_wv01</v>
       </c>
       <c r="J3">
@@ -799,7 +802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1</v>
       </c>
@@ -835,7 +838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1</v>
       </c>
@@ -871,7 +874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>1</v>
       </c>
@@ -907,7 +910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>1</v>
       </c>
@@ -943,7 +946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>1</v>
       </c>
@@ -982,7 +985,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1018,7 +1021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1055,7 +1058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1092,7 +1095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1129,7 +1132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1167,7 +1170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1204,7 +1207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1241,7 +1244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1278,7 +1281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1315,7 +1318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1352,7 +1355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1389,7 +1392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1426,7 +1429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1463,7 +1466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1500,7 +1503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1537,7 +1540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1574,7 +1577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1611,7 +1614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1648,7 +1651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1685,7 +1688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1725,7 +1728,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1765,7 +1768,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1802,7 +1805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1838,7 +1841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1877,7 +1880,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1913,7 +1916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>3</v>
       </c>
@@ -1950,7 +1953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>3</v>
       </c>
@@ -1987,7 +1990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>3</v>
       </c>
@@ -2024,7 +2027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>3</v>
       </c>
@@ -2061,7 +2064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>3</v>
       </c>
@@ -2098,7 +2101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A39">
         <v>3</v>
       </c>
@@ -2135,7 +2138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2172,7 +2175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>3</v>
       </c>
@@ -2209,7 +2212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2246,7 +2249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2283,7 +2286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A44">
         <v>3</v>
       </c>
@@ -2320,7 +2323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A45">
         <v>3</v>
       </c>
@@ -2357,7 +2360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A46">
         <v>3</v>
       </c>
@@ -2394,7 +2397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A47">
         <v>3</v>
       </c>
@@ -2431,7 +2434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A48">
         <v>3</v>
       </c>
@@ -2468,7 +2471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A49">
         <v>3</v>
       </c>
@@ -2505,7 +2508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>3</v>
       </c>
@@ -2542,7 +2545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A51">
         <v>3</v>
       </c>
@@ -2579,7 +2582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A52">
         <v>3</v>
       </c>
@@ -2616,7 +2619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A53">
         <v>3</v>
       </c>
@@ -2653,7 +2656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A54">
         <v>3</v>
       </c>
@@ -2690,7 +2693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A55">
         <v>3</v>
       </c>
@@ -2727,7 +2730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A56">
         <v>3</v>
       </c>
@@ -2764,7 +2767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A57">
         <v>3</v>
       </c>
@@ -2804,7 +2807,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A58">
         <v>3</v>
       </c>
@@ -2841,7 +2844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A59">
         <v>3</v>
       </c>
@@ -2877,7 +2880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A60">
         <v>3</v>
       </c>
@@ -2910,7 +2913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A61">
         <v>3</v>
       </c>
@@ -2943,7 +2946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A62">
         <v>3</v>
       </c>
@@ -2976,7 +2979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A63">
         <v>3</v>
       </c>
@@ -3009,7 +3012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A64">
         <v>3</v>
       </c>
@@ -3042,7 +3045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A65">
         <v>3</v>
       </c>
@@ -3075,7 +3078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A66">
         <v>3</v>
       </c>
@@ -3108,7 +3111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A67">
         <v>3</v>
       </c>
@@ -3141,7 +3144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A68">
         <v>3</v>
       </c>
@@ -3172,6 +3175,36 @@
       </c>
       <c r="J68">
         <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A69">
+        <v>3</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69" t="s">
+        <v>14</v>
+      </c>
+      <c r="D69">
+        <v>57</v>
+      </c>
+      <c r="E69" t="s">
+        <v>54</v>
+      </c>
+      <c r="F69">
+        <v>19</v>
+      </c>
+      <c r="G69" s="1">
+        <v>44316</v>
+      </c>
+      <c r="H69" t="s">
+        <v>93</v>
+      </c>
+      <c r="I69" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr57_20210430_pF_wv19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update week 71 uk
</commit_message>
<xml_diff>
--- a/data/spss_uk.xlsx
+++ b/data/spss_uk.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amygimma/lshtm/comix_data_clean/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AFF039F-225C-4F8A-A2DB-64ECB831296A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8231E9-8C9F-D848-857F-C67E32E79B71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2229" yWindow="2229" windowWidth="24685" windowHeight="13148" xr2:uid="{B6B7C775-E4A7-4345-8BD6-E691E151534C}"/>
+    <workbookView xWindow="2220" yWindow="2220" windowWidth="24680" windowHeight="13140" xr2:uid="{B6B7C775-E4A7-4345-8BD6-E691E151534C}"/>
   </bookViews>
   <sheets>
     <sheet name="UK" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="111">
   <si>
     <t>survey_version</t>
   </si>
@@ -361,6 +361,12 @@
   </si>
   <si>
     <t>21-037554_PFW25_Final_ICUO</t>
+  </si>
+  <si>
+    <t>21-037558_PEW26_Final_ICUO</t>
+  </si>
+  <si>
+    <t>21-037554_PFW26_Final_ICUO</t>
   </si>
 </sst>
 </file>
@@ -713,22 +719,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E8812C-49CD-4565-ACAD-8E318F9F9624}">
-  <dimension ref="A1:O82"/>
+  <dimension ref="A1:O84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="J82" sqref="J82"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="I88" sqref="I88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.3046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.3046875" customWidth="1"/>
-    <col min="7" max="7" width="10.69140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="58.3046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.3046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="58.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -775,7 +781,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -811,7 +817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -837,7 +843,7 @@
         <v>18</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I82" si="0">C3&amp;"_"&amp;"sr"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
+        <f t="shared" ref="I3:I84" si="0">C3&amp;"_"&amp;"sr"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
         <v>uk_sr02_20200214_pB_wv01</v>
       </c>
       <c r="J3">
@@ -847,7 +853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -883,7 +889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -919,7 +925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -955,7 +961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -991,7 +997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1030,7 +1036,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1066,7 +1072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1103,7 +1109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1140,7 +1146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1177,7 +1183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1215,7 +1221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1252,7 +1258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1289,7 +1295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1326,7 +1332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1363,7 +1369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1400,7 +1406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1437,7 +1443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1474,7 +1480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1511,7 +1517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1548,7 +1554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1585,7 +1591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1622,7 +1628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1659,7 +1665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1696,7 +1702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1733,7 +1739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1773,7 +1779,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1813,7 +1819,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1850,7 +1856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1886,7 +1892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1925,7 +1931,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1961,7 +1967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>3</v>
       </c>
@@ -1998,7 +2004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>3</v>
       </c>
@@ -2035,7 +2041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>3</v>
       </c>
@@ -2072,7 +2078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>3</v>
       </c>
@@ -2109,7 +2115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>3</v>
       </c>
@@ -2146,7 +2152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>3</v>
       </c>
@@ -2183,7 +2189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2220,7 +2226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>3</v>
       </c>
@@ -2257,7 +2263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2294,7 +2300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2331,7 +2337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>3</v>
       </c>
@@ -2368,7 +2374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>3</v>
       </c>
@@ -2405,7 +2411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>3</v>
       </c>
@@ -2442,7 +2448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>3</v>
       </c>
@@ -2479,7 +2485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>3</v>
       </c>
@@ -2516,7 +2522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>3</v>
       </c>
@@ -2553,7 +2559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>3</v>
       </c>
@@ -2590,7 +2596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>3</v>
       </c>
@@ -2627,7 +2633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>3</v>
       </c>
@@ -2664,7 +2670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>3</v>
       </c>
@@ -2701,7 +2707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>3</v>
       </c>
@@ -2738,7 +2744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>3</v>
       </c>
@@ -2775,7 +2781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>3</v>
       </c>
@@ -2812,7 +2818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>3</v>
       </c>
@@ -2852,7 +2858,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>3</v>
       </c>
@@ -2889,7 +2895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>3</v>
       </c>
@@ -2925,7 +2931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>3</v>
       </c>
@@ -2958,7 +2964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>3</v>
       </c>
@@ -2991,7 +2997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>3</v>
       </c>
@@ -3024,7 +3030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>3</v>
       </c>
@@ -3057,7 +3063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>3</v>
       </c>
@@ -3090,7 +3096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>3</v>
       </c>
@@ -3123,7 +3129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>3</v>
       </c>
@@ -3156,7 +3162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>3</v>
       </c>
@@ -3189,7 +3195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>3</v>
       </c>
@@ -3222,7 +3228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>3</v>
       </c>
@@ -3255,7 +3261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>3</v>
       </c>
@@ -3288,7 +3294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>3</v>
       </c>
@@ -3321,7 +3327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>3</v>
       </c>
@@ -3354,7 +3360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>3</v>
       </c>
@@ -3387,7 +3393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>3</v>
       </c>
@@ -3420,7 +3426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>3</v>
       </c>
@@ -3453,7 +3459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>3</v>
       </c>
@@ -3486,7 +3492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>3</v>
       </c>
@@ -3519,7 +3525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>3</v>
       </c>
@@ -3552,7 +3558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>3</v>
       </c>
@@ -3585,7 +3591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>3</v>
       </c>
@@ -3618,7 +3624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>3</v>
       </c>
@@ -3651,7 +3657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>3</v>
       </c>
@@ -3682,6 +3688,66 @@
       </c>
       <c r="J82">
         <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>3</v>
+      </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
+      <c r="C83" t="s">
+        <v>14</v>
+      </c>
+      <c r="D83">
+        <v>70</v>
+      </c>
+      <c r="E83" t="s">
+        <v>51</v>
+      </c>
+      <c r="F83">
+        <v>26</v>
+      </c>
+      <c r="G83" s="1">
+        <v>44407</v>
+      </c>
+      <c r="H83" t="s">
+        <v>109</v>
+      </c>
+      <c r="I83" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr70_20210730_pE_wv26</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>3</v>
+      </c>
+      <c r="B84">
+        <v>0</v>
+      </c>
+      <c r="C84" t="s">
+        <v>14</v>
+      </c>
+      <c r="D84">
+        <v>71</v>
+      </c>
+      <c r="E84" t="s">
+        <v>54</v>
+      </c>
+      <c r="F84">
+        <v>26</v>
+      </c>
+      <c r="G84" s="1">
+        <v>44413</v>
+      </c>
+      <c r="H84" t="s">
+        <v>110</v>
+      </c>
+      <c r="I84" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr71_20210805_pF_wv26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for survey round 72
</commit_message>
<xml_diff>
--- a/data/spss_uk.xlsx
+++ b/data/spss_uk.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AFF039F-225C-4F8A-A2DB-64ECB831296A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4FD8EC-27A7-4335-9D49-BC4121B38F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2229" yWindow="2229" windowWidth="24685" windowHeight="13148" xr2:uid="{B6B7C775-E4A7-4345-8BD6-E691E151534C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6B7C775-E4A7-4345-8BD6-E691E151534C}"/>
   </bookViews>
   <sheets>
     <sheet name="UK" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="112">
   <si>
     <t>survey_version</t>
   </si>
@@ -361,6 +361,15 @@
   </si>
   <si>
     <t>21-037554_PFW25_Final_ICUO</t>
+  </si>
+  <si>
+    <t>21-037558_PEW26_Final_ICUO</t>
+  </si>
+  <si>
+    <t>21-037554_PFW26_Final_ICUO</t>
+  </si>
+  <si>
+    <t>21-037558_PEW27_Final_ICUO</t>
   </si>
 </sst>
 </file>
@@ -713,22 +722,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E8812C-49CD-4565-ACAD-8E318F9F9624}">
-  <dimension ref="A1:O82"/>
+  <dimension ref="A1:O85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="J82" sqref="J82"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="J85" sqref="A85:J85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.3046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.3046875" customWidth="1"/>
-    <col min="7" max="7" width="10.69140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="58.3046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.3046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="58.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -775,7 +784,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -811,7 +820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -847,7 +856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -883,7 +892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -919,7 +928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -955,7 +964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -991,7 +1000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1030,7 +1039,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1066,7 +1075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1103,7 +1112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1140,7 +1149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1177,7 +1186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1215,7 +1224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1252,7 +1261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1289,7 +1298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1326,7 +1335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1363,7 +1372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1400,7 +1409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1437,7 +1446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1474,7 +1483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1511,7 +1520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1548,7 +1557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1585,7 +1594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1622,7 +1631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1659,7 +1668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1696,7 +1705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1733,7 +1742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1773,7 +1782,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1813,7 +1822,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1850,7 +1859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1886,7 +1895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1925,7 +1934,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1961,7 +1970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3</v>
       </c>
@@ -1998,7 +2007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3</v>
       </c>
@@ -2035,7 +2044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>3</v>
       </c>
@@ -2072,7 +2081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>3</v>
       </c>
@@ -2109,7 +2118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3</v>
       </c>
@@ -2146,7 +2155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3</v>
       </c>
@@ -2183,7 +2192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2220,7 +2229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>3</v>
       </c>
@@ -2257,7 +2266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2294,7 +2303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2331,7 +2340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>3</v>
       </c>
@@ -2368,7 +2377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>3</v>
       </c>
@@ -2405,7 +2414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>3</v>
       </c>
@@ -2442,7 +2451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>3</v>
       </c>
@@ -2479,7 +2488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>3</v>
       </c>
@@ -2516,7 +2525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>3</v>
       </c>
@@ -2553,7 +2562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>3</v>
       </c>
@@ -2590,7 +2599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>3</v>
       </c>
@@ -2627,7 +2636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>3</v>
       </c>
@@ -2664,7 +2673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>3</v>
       </c>
@@ -2701,7 +2710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>3</v>
       </c>
@@ -2738,7 +2747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>3</v>
       </c>
@@ -2775,7 +2784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>3</v>
       </c>
@@ -2812,7 +2821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>3</v>
       </c>
@@ -2852,7 +2861,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>3</v>
       </c>
@@ -2889,7 +2898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>3</v>
       </c>
@@ -2925,7 +2934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>3</v>
       </c>
@@ -2958,7 +2967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>3</v>
       </c>
@@ -2991,7 +3000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>3</v>
       </c>
@@ -3024,7 +3033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>3</v>
       </c>
@@ -3057,7 +3066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>3</v>
       </c>
@@ -3090,7 +3099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>3</v>
       </c>
@@ -3123,7 +3132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>3</v>
       </c>
@@ -3156,7 +3165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>3</v>
       </c>
@@ -3189,7 +3198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>3</v>
       </c>
@@ -3222,7 +3231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>3</v>
       </c>
@@ -3255,7 +3264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>3</v>
       </c>
@@ -3288,7 +3297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>3</v>
       </c>
@@ -3321,7 +3330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>3</v>
       </c>
@@ -3354,7 +3363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>3</v>
       </c>
@@ -3387,7 +3396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>3</v>
       </c>
@@ -3420,7 +3429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>3</v>
       </c>
@@ -3453,7 +3462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>3</v>
       </c>
@@ -3486,7 +3495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>3</v>
       </c>
@@ -3519,7 +3528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>3</v>
       </c>
@@ -3552,7 +3561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>3</v>
       </c>
@@ -3585,7 +3594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>3</v>
       </c>
@@ -3618,7 +3627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>3</v>
       </c>
@@ -3651,7 +3660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>3</v>
       </c>
@@ -3681,6 +3690,105 @@
         <v>uk_sr69_20210722_pF_wv25</v>
       </c>
       <c r="J82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>3</v>
+      </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
+      <c r="C83" t="s">
+        <v>14</v>
+      </c>
+      <c r="D83">
+        <v>70</v>
+      </c>
+      <c r="E83" t="s">
+        <v>51</v>
+      </c>
+      <c r="F83">
+        <v>26</v>
+      </c>
+      <c r="G83" s="1">
+        <v>44407</v>
+      </c>
+      <c r="H83" t="s">
+        <v>109</v>
+      </c>
+      <c r="I83" t="str">
+        <f t="shared" ref="I83:I85" si="5">C83&amp;"_"&amp;"sr"&amp;TEXT(D83,"00")&amp;"_"&amp;YEAR(G83)&amp;TEXT(G83,"MM")&amp;TEXT(G83,"DD")&amp;"_p"&amp;E83&amp;"_wv"&amp;TEXT(F83,"00")&amp;""</f>
+        <v>uk_sr70_20210730_pE_wv26</v>
+      </c>
+      <c r="J83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>3</v>
+      </c>
+      <c r="B84">
+        <v>0</v>
+      </c>
+      <c r="C84" t="s">
+        <v>14</v>
+      </c>
+      <c r="D84">
+        <v>71</v>
+      </c>
+      <c r="E84" t="s">
+        <v>54</v>
+      </c>
+      <c r="F84">
+        <v>26</v>
+      </c>
+      <c r="G84" s="1">
+        <v>44413</v>
+      </c>
+      <c r="H84" t="s">
+        <v>110</v>
+      </c>
+      <c r="I84" t="str">
+        <f t="shared" si="5"/>
+        <v>uk_sr71_20210805_pF_wv26</v>
+      </c>
+      <c r="J84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>3</v>
+      </c>
+      <c r="B85">
+        <v>0</v>
+      </c>
+      <c r="C85" t="s">
+        <v>14</v>
+      </c>
+      <c r="D85">
+        <v>72</v>
+      </c>
+      <c r="E85" t="s">
+        <v>51</v>
+      </c>
+      <c r="F85">
+        <v>27</v>
+      </c>
+      <c r="G85" s="1">
+        <v>44420</v>
+      </c>
+      <c r="H85" t="s">
+        <v>111</v>
+      </c>
+      <c r="I85" t="str">
+        <f t="shared" si="5"/>
+        <v>uk_sr72_20210812_pE_wv27</v>
+      </c>
+      <c r="J85">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updates for running locally - ag
</commit_message>
<xml_diff>
--- a/data/spss_uk.xlsx
+++ b/data/spss_uk.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amygimma/lshtm/comix_data_clean/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4FD8EC-27A7-4335-9D49-BC4121B38F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BDD58D8-E519-C042-A5A2-C53BB79BDF05}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6B7C775-E4A7-4345-8BD6-E691E151534C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{B6B7C775-E4A7-4345-8BD6-E691E151534C}"/>
   </bookViews>
   <sheets>
     <sheet name="UK" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="114">
   <si>
     <t>survey_version</t>
   </si>
@@ -370,6 +370,12 @@
   </si>
   <si>
     <t>21-037558_PEW27_Final_ICUO</t>
+  </si>
+  <si>
+    <t>21-037554_PFW27_Final_ICUO</t>
+  </si>
+  <si>
+    <t>21-037558_PEW28_Final_ICUO</t>
   </si>
 </sst>
 </file>
@@ -722,22 +728,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E8812C-49CD-4565-ACAD-8E318F9F9624}">
-  <dimension ref="A1:O85"/>
+  <dimension ref="A1:O87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="J85" sqref="A85:J85"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="J89" sqref="J89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="58.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="58.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -784,7 +790,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -820,7 +826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -856,7 +862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -892,7 +898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -928,7 +934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -964,7 +970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1000,7 +1006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1039,7 +1045,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1075,7 +1081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1112,7 +1118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1149,7 +1155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1186,7 +1192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1224,7 +1230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1261,7 +1267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1298,7 +1304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1335,7 +1341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1372,7 +1378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1409,7 +1415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1446,7 +1452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1483,7 +1489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1520,7 +1526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1557,7 +1563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1594,7 +1600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1631,7 +1637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1668,7 +1674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1705,7 +1711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1742,7 +1748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1782,7 +1788,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1822,7 +1828,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1859,7 +1865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1895,7 +1901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1934,7 +1940,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1970,7 +1976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>3</v>
       </c>
@@ -2007,7 +2013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>3</v>
       </c>
@@ -2044,7 +2050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>3</v>
       </c>
@@ -2081,7 +2087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>3</v>
       </c>
@@ -2118,7 +2124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>3</v>
       </c>
@@ -2155,7 +2161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>3</v>
       </c>
@@ -2192,7 +2198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2229,7 +2235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>3</v>
       </c>
@@ -2266,7 +2272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2303,7 +2309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2340,7 +2346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>3</v>
       </c>
@@ -2377,7 +2383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>3</v>
       </c>
@@ -2414,7 +2420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>3</v>
       </c>
@@ -2451,7 +2457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>3</v>
       </c>
@@ -2488,7 +2494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>3</v>
       </c>
@@ -2525,7 +2531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>3</v>
       </c>
@@ -2562,7 +2568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>3</v>
       </c>
@@ -2599,7 +2605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>3</v>
       </c>
@@ -2636,7 +2642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>3</v>
       </c>
@@ -2673,7 +2679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>3</v>
       </c>
@@ -2710,7 +2716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>3</v>
       </c>
@@ -2747,7 +2753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>3</v>
       </c>
@@ -2784,7 +2790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>3</v>
       </c>
@@ -2821,7 +2827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>3</v>
       </c>
@@ -2861,7 +2867,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>3</v>
       </c>
@@ -2898,7 +2904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>3</v>
       </c>
@@ -2934,7 +2940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>3</v>
       </c>
@@ -2967,7 +2973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>3</v>
       </c>
@@ -3000,7 +3006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>3</v>
       </c>
@@ -3033,7 +3039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>3</v>
       </c>
@@ -3066,7 +3072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>3</v>
       </c>
@@ -3099,7 +3105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>3</v>
       </c>
@@ -3132,7 +3138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>3</v>
       </c>
@@ -3165,7 +3171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>3</v>
       </c>
@@ -3198,7 +3204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>3</v>
       </c>
@@ -3231,7 +3237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>3</v>
       </c>
@@ -3264,7 +3270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>3</v>
       </c>
@@ -3297,7 +3303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>3</v>
       </c>
@@ -3330,7 +3336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>3</v>
       </c>
@@ -3363,7 +3369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>3</v>
       </c>
@@ -3396,7 +3402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>3</v>
       </c>
@@ -3429,7 +3435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>3</v>
       </c>
@@ -3462,7 +3468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>3</v>
       </c>
@@ -3495,7 +3501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>3</v>
       </c>
@@ -3528,7 +3534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>3</v>
       </c>
@@ -3561,7 +3567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>3</v>
       </c>
@@ -3594,7 +3600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>3</v>
       </c>
@@ -3627,7 +3633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>3</v>
       </c>
@@ -3660,7 +3666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>3</v>
       </c>
@@ -3693,7 +3699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>3</v>
       </c>
@@ -3719,14 +3725,14 @@
         <v>109</v>
       </c>
       <c r="I83" t="str">
-        <f t="shared" ref="I83:I85" si="5">C83&amp;"_"&amp;"sr"&amp;TEXT(D83,"00")&amp;"_"&amp;YEAR(G83)&amp;TEXT(G83,"MM")&amp;TEXT(G83,"DD")&amp;"_p"&amp;E83&amp;"_wv"&amp;TEXT(F83,"00")&amp;""</f>
+        <f t="shared" ref="I83:I87" si="5">C83&amp;"_"&amp;"sr"&amp;TEXT(D83,"00")&amp;"_"&amp;YEAR(G83)&amp;TEXT(G83,"MM")&amp;TEXT(G83,"DD")&amp;"_p"&amp;E83&amp;"_wv"&amp;TEXT(F83,"00")&amp;""</f>
         <v>uk_sr70_20210730_pE_wv26</v>
       </c>
       <c r="J83">
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>3</v>
       </c>
@@ -3759,7 +3765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>3</v>
       </c>
@@ -3790,6 +3796,69 @@
       </c>
       <c r="J85">
         <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>3</v>
+      </c>
+      <c r="B86">
+        <v>0</v>
+      </c>
+      <c r="C86" t="s">
+        <v>14</v>
+      </c>
+      <c r="D86">
+        <v>73</v>
+      </c>
+      <c r="E86" t="s">
+        <v>54</v>
+      </c>
+      <c r="F86">
+        <v>27</v>
+      </c>
+      <c r="G86" s="1">
+        <v>44427</v>
+      </c>
+      <c r="H86" t="s">
+        <v>112</v>
+      </c>
+      <c r="I86" t="str">
+        <f t="shared" si="5"/>
+        <v>uk_sr73_20210819_pF_wv27</v>
+      </c>
+      <c r="J86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>3</v>
+      </c>
+      <c r="B87">
+        <v>0</v>
+      </c>
+      <c r="C87" t="s">
+        <v>14</v>
+      </c>
+      <c r="D87">
+        <v>74</v>
+      </c>
+      <c r="E87" t="s">
+        <v>51</v>
+      </c>
+      <c r="F87">
+        <v>28</v>
+      </c>
+      <c r="G87" s="1">
+        <v>44434</v>
+      </c>
+      <c r="H87" t="s">
+        <v>113</v>
+      </c>
+      <c r="I87" t="str">
+        <f t="shared" si="5"/>
+        <v>uk_sr74_20210826_pE_wv28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add round 94 to spreadsheet
</commit_message>
<xml_diff>
--- a/data/spss_uk.xlsx
+++ b/data/spss_uk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68167CD1-7AE4-4F5E-BF0A-E501A83117F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2568D9FC-AB82-4559-89BA-C614F1B1E5CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{B6B7C775-E4A7-4345-8BD6-E691E151534C}"/>
+    <workbookView xWindow="720" yWindow="720" windowWidth="24686" windowHeight="13191" xr2:uid="{B6B7C775-E4A7-4345-8BD6-E691E151534C}"/>
   </bookViews>
   <sheets>
     <sheet name="UK" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="134">
   <si>
     <t>survey_version</t>
   </si>
@@ -433,6 +433,9 @@
   </si>
   <si>
     <t>21-088071_PFW37_Final_ICUO</t>
+  </si>
+  <si>
+    <t>21-088043_PEW38_Final_ICUO</t>
   </si>
 </sst>
 </file>
@@ -785,10 +788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E8812C-49CD-4565-ACAD-8E318F9F9624}">
-  <dimension ref="A1:O106"/>
+  <dimension ref="A1:O107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="K106" sqref="K106"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="L107" sqref="L107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3851,7 +3854,7 @@
         <v>109</v>
       </c>
       <c r="I83" t="str">
-        <f t="shared" ref="I83:I106" si="5">C83&amp;"_"&amp;"sr"&amp;TEXT(D83,"00")&amp;"_"&amp;YEAR(G83)&amp;TEXT(G83,"MM")&amp;TEXT(G83,"DD")&amp;"_p"&amp;E83&amp;"_wv"&amp;TEXT(F83,"00")&amp;""</f>
+        <f t="shared" ref="I83:I107" si="5">C83&amp;"_"&amp;"sr"&amp;TEXT(D83,"00")&amp;"_"&amp;YEAR(G83)&amp;TEXT(G83,"MM")&amp;TEXT(G83,"DD")&amp;"_p"&amp;E83&amp;"_wv"&amp;TEXT(F83,"00")&amp;""</f>
         <v>uk_sr70_20210730_pE_wv26</v>
       </c>
       <c r="J83">
@@ -4686,6 +4689,42 @@
         <v>1</v>
       </c>
       <c r="K106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A107">
+        <v>8</v>
+      </c>
+      <c r="B107">
+        <v>0</v>
+      </c>
+      <c r="C107" t="s">
+        <v>14</v>
+      </c>
+      <c r="D107">
+        <v>94</v>
+      </c>
+      <c r="E107" t="s">
+        <v>51</v>
+      </c>
+      <c r="F107">
+        <v>38</v>
+      </c>
+      <c r="G107" s="1">
+        <v>44574</v>
+      </c>
+      <c r="H107" t="s">
+        <v>133</v>
+      </c>
+      <c r="I107" t="str">
+        <f t="shared" si="5"/>
+        <v>uk_sr94_20220113_pE_wv38</v>
+      </c>
+      <c r="J107">
+        <v>1</v>
+      </c>
+      <c r="K107">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update for SR 96
</commit_message>
<xml_diff>
--- a/data/spss_uk.xlsx
+++ b/data/spss_uk.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amygimma/lshtm/comix_data_clean/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F98DD7-85D7-0D4F-A27F-55D3FF41A154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C869A3-6301-456D-9FC0-B804A0066303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="720" windowWidth="24680" windowHeight="13200" xr2:uid="{B6B7C775-E4A7-4345-8BD6-E691E151534C}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{B6B7C775-E4A7-4345-8BD6-E691E151534C}"/>
   </bookViews>
   <sheets>
     <sheet name="UK" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="136">
   <si>
     <t>survey_version</t>
   </si>
@@ -439,6 +439,9 @@
   </si>
   <si>
     <t>21-088071_PFW38_Final_ICUO</t>
+  </si>
+  <si>
+    <t>21-088071_PFW39_Final_ICUO</t>
   </si>
 </sst>
 </file>
@@ -791,22 +794,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E8812C-49CD-4565-ACAD-8E318F9F9624}">
-  <dimension ref="A1:O108"/>
+  <dimension ref="A1:O109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="C111" sqref="C111"/>
+      <selection activeCell="J108" sqref="J108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="58.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3046875" customWidth="1"/>
+    <col min="7" max="7" width="10.69140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="58.3046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -853,7 +856,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -889,7 +892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -925,7 +928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1</v>
       </c>
@@ -961,7 +964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1</v>
       </c>
@@ -997,7 +1000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1033,7 +1036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1069,7 +1072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1108,7 +1111,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1144,7 +1147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1181,7 +1184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1218,7 +1221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1255,7 +1258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1293,7 +1296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1330,7 +1333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1367,7 +1370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1404,7 +1407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1441,7 +1444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1478,7 +1481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1515,7 +1518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1552,7 +1555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1589,7 +1592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1626,7 +1629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1663,7 +1666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1700,7 +1703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1737,7 +1740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1774,7 +1777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1811,7 +1814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1851,7 +1854,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1891,7 +1894,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1928,7 +1931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1964,7 +1967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>3</v>
       </c>
@@ -2003,7 +2006,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>3</v>
       </c>
@@ -2039,7 +2042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>3</v>
       </c>
@@ -2076,7 +2079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>3</v>
       </c>
@@ -2113,7 +2116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>3</v>
       </c>
@@ -2150,7 +2153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>3</v>
       </c>
@@ -2187,7 +2190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>3</v>
       </c>
@@ -2224,7 +2227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A39">
         <v>3</v>
       </c>
@@ -2261,7 +2264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2298,7 +2301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>3</v>
       </c>
@@ -2335,7 +2338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2372,7 +2375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2409,7 +2412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A44">
         <v>3</v>
       </c>
@@ -2446,7 +2449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A45">
         <v>3</v>
       </c>
@@ -2483,7 +2486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A46">
         <v>3</v>
       </c>
@@ -2520,7 +2523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A47">
         <v>3</v>
       </c>
@@ -2557,7 +2560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A48">
         <v>3</v>
       </c>
@@ -2594,7 +2597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A49">
         <v>3</v>
       </c>
@@ -2631,7 +2634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>3</v>
       </c>
@@ -2668,7 +2671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A51">
         <v>3</v>
       </c>
@@ -2705,7 +2708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A52">
         <v>3</v>
       </c>
@@ -2742,7 +2745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A53">
         <v>3</v>
       </c>
@@ -2779,7 +2782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A54">
         <v>3</v>
       </c>
@@ -2816,7 +2819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A55">
         <v>3</v>
       </c>
@@ -2853,7 +2856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A56">
         <v>3</v>
       </c>
@@ -2890,7 +2893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A57">
         <v>3</v>
       </c>
@@ -2930,7 +2933,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A58">
         <v>3</v>
       </c>
@@ -2967,7 +2970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A59">
         <v>3</v>
       </c>
@@ -3003,7 +3006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A60">
         <v>3</v>
       </c>
@@ -3039,7 +3042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A61">
         <v>3</v>
       </c>
@@ -3075,7 +3078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A62">
         <v>3</v>
       </c>
@@ -3111,7 +3114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A63">
         <v>3</v>
       </c>
@@ -3147,7 +3150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A64">
         <v>3</v>
       </c>
@@ -3183,7 +3186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A65">
         <v>3</v>
       </c>
@@ -3219,7 +3222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A66">
         <v>3</v>
       </c>
@@ -3255,7 +3258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A67">
         <v>3</v>
       </c>
@@ -3291,7 +3294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A68">
         <v>3</v>
       </c>
@@ -3327,7 +3330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A69">
         <v>3</v>
       </c>
@@ -3363,7 +3366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A70">
         <v>3</v>
       </c>
@@ -3399,7 +3402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A71">
         <v>3</v>
       </c>
@@ -3435,7 +3438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A72">
         <v>3</v>
       </c>
@@ -3471,7 +3474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A73">
         <v>3</v>
       </c>
@@ -3507,7 +3510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A74">
         <v>3</v>
       </c>
@@ -3543,7 +3546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A75">
         <v>3</v>
       </c>
@@ -3579,7 +3582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A76">
         <v>3</v>
       </c>
@@ -3615,7 +3618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A77">
         <v>3</v>
       </c>
@@ -3651,7 +3654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A78">
         <v>3</v>
       </c>
@@ -3687,7 +3690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A79">
         <v>3</v>
       </c>
@@ -3723,7 +3726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A80">
         <v>3</v>
       </c>
@@ -3759,7 +3762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A81">
         <v>3</v>
       </c>
@@ -3795,7 +3798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A82">
         <v>3</v>
       </c>
@@ -3831,7 +3834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A83">
         <v>3</v>
       </c>
@@ -3857,7 +3860,7 @@
         <v>109</v>
       </c>
       <c r="I83" t="str">
-        <f t="shared" ref="I83:I108" si="5">C83&amp;"_"&amp;"sr"&amp;TEXT(D83,"00")&amp;"_"&amp;YEAR(G83)&amp;TEXT(G83,"MM")&amp;TEXT(G83,"DD")&amp;"_p"&amp;E83&amp;"_wv"&amp;TEXT(F83,"00")&amp;""</f>
+        <f t="shared" ref="I83:I109" si="5">C83&amp;"_"&amp;"sr"&amp;TEXT(D83,"00")&amp;"_"&amp;YEAR(G83)&amp;TEXT(G83,"MM")&amp;TEXT(G83,"DD")&amp;"_p"&amp;E83&amp;"_wv"&amp;TEXT(F83,"00")&amp;""</f>
         <v>uk_sr70_20210730_pE_wv26</v>
       </c>
       <c r="J83">
@@ -3867,7 +3870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A84">
         <v>3</v>
       </c>
@@ -3903,7 +3906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A85">
         <v>3</v>
       </c>
@@ -3939,7 +3942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A86">
         <v>3</v>
       </c>
@@ -3975,7 +3978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A87">
         <v>3</v>
       </c>
@@ -4011,7 +4014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A88">
         <v>3</v>
       </c>
@@ -4047,7 +4050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A89">
         <v>3</v>
       </c>
@@ -4083,7 +4086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A90">
         <v>3</v>
       </c>
@@ -4119,7 +4122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A91">
         <v>3</v>
       </c>
@@ -4155,7 +4158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A92">
         <v>3</v>
       </c>
@@ -4191,7 +4194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A93">
         <v>8</v>
       </c>
@@ -4227,7 +4230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A94">
         <v>8</v>
       </c>
@@ -4263,7 +4266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A95">
         <v>8</v>
       </c>
@@ -4299,7 +4302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A96">
         <v>8</v>
       </c>
@@ -4335,7 +4338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A97">
         <v>8</v>
       </c>
@@ -4371,7 +4374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A98">
         <v>8</v>
       </c>
@@ -4407,7 +4410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A99">
         <v>8</v>
       </c>
@@ -4443,7 +4446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A100">
         <v>8</v>
       </c>
@@ -4479,7 +4482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A101">
         <v>8</v>
       </c>
@@ -4515,7 +4518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A102">
         <v>8</v>
       </c>
@@ -4551,7 +4554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A103">
         <v>8</v>
       </c>
@@ -4587,7 +4590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A104">
         <v>8</v>
       </c>
@@ -4623,7 +4626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A105">
         <v>8</v>
       </c>
@@ -4659,7 +4662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A106">
         <v>8</v>
       </c>
@@ -4695,7 +4698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A107">
         <v>8</v>
       </c>
@@ -4731,9 +4734,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A108">
         <v>8</v>
+      </c>
+      <c r="B108">
+        <v>0</v>
       </c>
       <c r="C108" t="s">
         <v>14</v>
@@ -4756,6 +4762,48 @@
       <c r="I108" t="str">
         <f t="shared" si="5"/>
         <v>uk_sr95_20220121_pF_wv38</v>
+      </c>
+      <c r="J108">
+        <v>1</v>
+      </c>
+      <c r="K108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A109">
+        <v>8</v>
+      </c>
+      <c r="B109">
+        <v>0</v>
+      </c>
+      <c r="C109" t="s">
+        <v>14</v>
+      </c>
+      <c r="D109">
+        <v>96</v>
+      </c>
+      <c r="E109" t="s">
+        <v>51</v>
+      </c>
+      <c r="F109">
+        <v>39</v>
+      </c>
+      <c r="G109" s="1">
+        <v>44596</v>
+      </c>
+      <c r="H109" t="s">
+        <v>135</v>
+      </c>
+      <c r="I109" t="str">
+        <f t="shared" si="5"/>
+        <v>uk_sr96_20220204_pE_wv39</v>
+      </c>
+      <c r="J109">
+        <v>1</v>
+      </c>
+      <c r="K109">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for round 99
</commit_message>
<xml_diff>
--- a/data/spss_uk.xlsx
+++ b/data/spss_uk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C869A3-6301-456D-9FC0-B804A0066303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7A3D50-6859-465F-964B-25F0FD5E6A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{B6B7C775-E4A7-4345-8BD6-E691E151534C}"/>
+    <workbookView xWindow="2126" yWindow="2803" windowWidth="24685" windowHeight="13191" xr2:uid="{B6B7C775-E4A7-4345-8BD6-E691E151534C}"/>
   </bookViews>
   <sheets>
     <sheet name="UK" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="139">
   <si>
     <t>survey_version</t>
   </si>
@@ -442,6 +442,15 @@
   </si>
   <si>
     <t>21-088071_PFW39_Final_ICUO</t>
+  </si>
+  <si>
+    <t>21-088043_PEW39_Final_ICUO</t>
+  </si>
+  <si>
+    <t>21-088043_PEW40_Final_ICUO</t>
+  </si>
+  <si>
+    <t>21-088071_PFW40_Final_ICUO</t>
   </si>
 </sst>
 </file>
@@ -794,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E8812C-49CD-4565-ACAD-8E318F9F9624}">
-  <dimension ref="A1:O109"/>
+  <dimension ref="A1:O112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="J108" sqref="J108"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="I112" sqref="I112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3860,7 +3869,7 @@
         <v>109</v>
       </c>
       <c r="I83" t="str">
-        <f t="shared" ref="I83:I109" si="5">C83&amp;"_"&amp;"sr"&amp;TEXT(D83,"00")&amp;"_"&amp;YEAR(G83)&amp;TEXT(G83,"MM")&amp;TEXT(G83,"DD")&amp;"_p"&amp;E83&amp;"_wv"&amp;TEXT(F83,"00")&amp;""</f>
+        <f t="shared" ref="I83:I112" si="5">C83&amp;"_"&amp;"sr"&amp;TEXT(D83,"00")&amp;"_"&amp;YEAR(G83)&amp;TEXT(G83,"MM")&amp;TEXT(G83,"DD")&amp;"_p"&amp;E83&amp;"_wv"&amp;TEXT(F83,"00")&amp;""</f>
         <v>uk_sr70_20210730_pE_wv26</v>
       </c>
       <c r="J83">
@@ -4790,19 +4799,127 @@
         <v>39</v>
       </c>
       <c r="G109" s="1">
-        <v>44596</v>
+        <v>44592</v>
       </c>
       <c r="H109" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I109" t="str">
         <f t="shared" si="5"/>
-        <v>uk_sr96_20220204_pE_wv39</v>
+        <v>uk_sr96_20220131_pE_wv39</v>
       </c>
       <c r="J109">
         <v>1</v>
       </c>
       <c r="K109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A110">
+        <v>8</v>
+      </c>
+      <c r="B110">
+        <v>0</v>
+      </c>
+      <c r="C110" t="s">
+        <v>14</v>
+      </c>
+      <c r="D110">
+        <v>97</v>
+      </c>
+      <c r="E110" t="s">
+        <v>54</v>
+      </c>
+      <c r="F110">
+        <v>39</v>
+      </c>
+      <c r="G110" s="1">
+        <v>44596</v>
+      </c>
+      <c r="H110" t="s">
+        <v>135</v>
+      </c>
+      <c r="I110" t="str">
+        <f t="shared" si="5"/>
+        <v>uk_sr97_20220204_pF_wv39</v>
+      </c>
+      <c r="J110">
+        <v>1</v>
+      </c>
+      <c r="K110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A111">
+        <v>8</v>
+      </c>
+      <c r="B111">
+        <v>0</v>
+      </c>
+      <c r="C111" t="s">
+        <v>14</v>
+      </c>
+      <c r="D111">
+        <v>98</v>
+      </c>
+      <c r="E111" t="s">
+        <v>51</v>
+      </c>
+      <c r="F111">
+        <v>40</v>
+      </c>
+      <c r="G111" s="1">
+        <v>44602</v>
+      </c>
+      <c r="H111" t="s">
+        <v>137</v>
+      </c>
+      <c r="I111" t="str">
+        <f t="shared" si="5"/>
+        <v>uk_sr98_20220210_pE_wv40</v>
+      </c>
+      <c r="J111">
+        <v>1</v>
+      </c>
+      <c r="K111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A112">
+        <v>8</v>
+      </c>
+      <c r="B112">
+        <v>0</v>
+      </c>
+      <c r="C112" t="s">
+        <v>14</v>
+      </c>
+      <c r="D112">
+        <v>99</v>
+      </c>
+      <c r="E112" t="s">
+        <v>54</v>
+      </c>
+      <c r="F112">
+        <v>40</v>
+      </c>
+      <c r="G112" s="1">
+        <v>44610</v>
+      </c>
+      <c r="H112" t="s">
+        <v>138</v>
+      </c>
+      <c r="I112" t="str">
+        <f t="shared" si="5"/>
+        <v>uk_sr99_20220218_pF_wv40</v>
+      </c>
+      <c r="J112">
+        <v>1</v>
+      </c>
+      <c r="K112">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update for round 101 - Last one for UK
</commit_message>
<xml_diff>
--- a/data/spss_uk.xlsx
+++ b/data/spss_uk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7A3D50-6859-465F-964B-25F0FD5E6A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B423CEF6-752B-4E8A-AC93-8D915CBC33B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2126" yWindow="2803" windowWidth="24685" windowHeight="13191" xr2:uid="{B6B7C775-E4A7-4345-8BD6-E691E151534C}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{B6B7C775-E4A7-4345-8BD6-E691E151534C}"/>
   </bookViews>
   <sheets>
     <sheet name="UK" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="141">
   <si>
     <t>survey_version</t>
   </si>
@@ -451,6 +451,12 @@
   </si>
   <si>
     <t>21-088071_PFW40_Final_ICUO</t>
+  </si>
+  <si>
+    <t>21-088043_PEW41_Final_ICUO</t>
+  </si>
+  <si>
+    <t>21-088071_PFW41_Final_ICUO</t>
   </si>
 </sst>
 </file>
@@ -803,10 +809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E8812C-49CD-4565-ACAD-8E318F9F9624}">
-  <dimension ref="A1:O112"/>
+  <dimension ref="A1:O114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="I112" sqref="I112"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="H86" sqref="H86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3869,7 +3875,7 @@
         <v>109</v>
       </c>
       <c r="I83" t="str">
-        <f t="shared" ref="I83:I112" si="5">C83&amp;"_"&amp;"sr"&amp;TEXT(D83,"00")&amp;"_"&amp;YEAR(G83)&amp;TEXT(G83,"MM")&amp;TEXT(G83,"DD")&amp;"_p"&amp;E83&amp;"_wv"&amp;TEXT(F83,"00")&amp;""</f>
+        <f t="shared" ref="I83:I114" si="5">C83&amp;"_"&amp;"sr"&amp;TEXT(D83,"00")&amp;"_"&amp;YEAR(G83)&amp;TEXT(G83,"MM")&amp;TEXT(G83,"DD")&amp;"_p"&amp;E83&amp;"_wv"&amp;TEXT(F83,"00")&amp;""</f>
         <v>uk_sr70_20210730_pE_wv26</v>
       </c>
       <c r="J83">
@@ -4920,6 +4926,78 @@
         <v>1</v>
       </c>
       <c r="K112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A113">
+        <v>8</v>
+      </c>
+      <c r="B113">
+        <v>0</v>
+      </c>
+      <c r="C113" t="s">
+        <v>14</v>
+      </c>
+      <c r="D113">
+        <v>100</v>
+      </c>
+      <c r="E113" t="s">
+        <v>51</v>
+      </c>
+      <c r="F113">
+        <v>41</v>
+      </c>
+      <c r="G113" s="1">
+        <v>44617</v>
+      </c>
+      <c r="H113" t="s">
+        <v>139</v>
+      </c>
+      <c r="I113" t="str">
+        <f t="shared" si="5"/>
+        <v>uk_sr100_20220225_pE_wv41</v>
+      </c>
+      <c r="J113">
+        <v>1</v>
+      </c>
+      <c r="K113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A114">
+        <v>8</v>
+      </c>
+      <c r="B114">
+        <v>0</v>
+      </c>
+      <c r="C114" t="s">
+        <v>14</v>
+      </c>
+      <c r="D114">
+        <v>101</v>
+      </c>
+      <c r="E114" t="s">
+        <v>54</v>
+      </c>
+      <c r="F114">
+        <v>41</v>
+      </c>
+      <c r="G114" s="1">
+        <v>44624</v>
+      </c>
+      <c r="H114" t="s">
+        <v>140</v>
+      </c>
+      <c r="I114" t="str">
+        <f t="shared" si="5"/>
+        <v>uk_sr101_20220304_pF_wv41</v>
+      </c>
+      <c r="J114">
+        <v>1</v>
+      </c>
+      <c r="K114">
         <v>1</v>
       </c>
     </row>

</xml_diff>